<commit_message>
Se hace una limpieza de datos del dataframe original en el analisis de datos. Aquí se eliminan cosas como los movimientos entre escenarios o eventos en los menus que solo son ruido
</commit_message>
<xml_diff>
--- a/data_analysis/db_env/app/results/global.xlsx
+++ b/data_analysis/db_env/app/results/global.xlsx
@@ -1129,7 +1129,7 @@
         <v>49.8</v>
       </c>
       <c r="BQ2" t="n">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="BR2" t="n">
         <v>170</v>
@@ -1141,13 +1141,13 @@
         <v>0</v>
       </c>
       <c r="BU2" t="n">
-        <v>484.17</v>
+        <v>207.1</v>
       </c>
       <c r="BV2" t="n">
         <v>30.5</v>
       </c>
       <c r="BW2" t="n">
-        <v>365</v>
+        <v>321</v>
       </c>
       <c r="BX2" t="n">
         <v>0</v>
@@ -1159,10 +1159,10 @@
         <v>36</v>
       </c>
       <c r="CA2" t="n">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="CB2" t="n">
-        <v>82</v>
+        <v>40</v>
       </c>
       <c r="CC2" t="n">
         <v>6</v>
@@ -1171,7 +1171,7 @@
         <v>32</v>
       </c>
       <c r="CE2" t="n">
-        <v>2.61</v>
+        <v>2.08</v>
       </c>
       <c r="CF2" t="n">
         <v>13.36</v>
@@ -1180,19 +1180,19 @@
         <v>0.55</v>
       </c>
       <c r="CH2" t="n">
-        <v>7.91</v>
+        <v>7.82</v>
       </c>
       <c r="CI2" t="n">
         <v>15.45</v>
       </c>
       <c r="CJ2" t="n">
-        <v>44.02</v>
+        <v>18.83</v>
       </c>
       <c r="CK2" t="n">
         <v>2.77</v>
       </c>
       <c r="CL2" t="n">
-        <v>33.18</v>
+        <v>29.18</v>
       </c>
       <c r="CM2" t="n">
         <v>0</v>
@@ -1204,10 +1204,10 @@
         <v>3.27</v>
       </c>
       <c r="CP2" t="n">
-        <v>4.36</v>
+        <v>4.18</v>
       </c>
       <c r="CQ2" t="n">
-        <v>7.45</v>
+        <v>3.64</v>
       </c>
       <c r="CR2" t="n">
         <v>0.55</v>
@@ -1430,7 +1430,7 @@
         <v>95</v>
       </c>
       <c r="BQ3" t="n">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="BR3" t="n">
         <v>153</v>
@@ -1442,7 +1442,7 @@
         <v>0</v>
       </c>
       <c r="BU3" t="n">
-        <v>533.5599999999999</v>
+        <v>253.09</v>
       </c>
       <c r="BV3" t="n">
         <v>23.74</v>
@@ -1481,13 +1481,13 @@
         <v>0.36</v>
       </c>
       <c r="CH3" t="n">
-        <v>6.55</v>
+        <v>6.45</v>
       </c>
       <c r="CI3" t="n">
         <v>13.91</v>
       </c>
       <c r="CJ3" t="n">
-        <v>48.51</v>
+        <v>23.01</v>
       </c>
       <c r="CK3" t="n">
         <v>2.16</v>
@@ -1749,31 +1749,31 @@
         <v>22.37</v>
       </c>
       <c r="BW4" t="n">
-        <v>423</v>
+        <v>225</v>
       </c>
       <c r="BX4" t="n">
         <v>0</v>
       </c>
       <c r="BY4" t="n">
-        <v>29</v>
+        <v>2</v>
       </c>
       <c r="BZ4" t="n">
-        <v>148</v>
+        <v>118</v>
       </c>
       <c r="CA4" t="n">
+        <v>0</v>
+      </c>
+      <c r="CB4" t="n">
         <v>16</v>
       </c>
-      <c r="CB4" t="n">
-        <v>129</v>
-      </c>
       <c r="CC4" t="n">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="CD4" t="n">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="CE4" t="n">
-        <v>627.0700000000001</v>
+        <v>1.51</v>
       </c>
       <c r="CF4" t="n">
         <v>17.27</v>
@@ -1794,28 +1794,28 @@
         <v>2.03</v>
       </c>
       <c r="CL4" t="n">
-        <v>38.45</v>
+        <v>20.45</v>
       </c>
       <c r="CM4" t="n">
         <v>0</v>
       </c>
       <c r="CN4" t="n">
-        <v>2.64</v>
+        <v>0.18</v>
       </c>
       <c r="CO4" t="n">
-        <v>13.45</v>
+        <v>10.73</v>
       </c>
       <c r="CP4" t="n">
+        <v>0</v>
+      </c>
+      <c r="CQ4" t="n">
         <v>1.45</v>
       </c>
-      <c r="CQ4" t="n">
-        <v>11.73</v>
-      </c>
       <c r="CR4" t="n">
-        <v>3.73</v>
+        <v>3.18</v>
       </c>
       <c r="CS4" t="n">
-        <v>5.27</v>
+        <v>4.91</v>
       </c>
     </row>
     <row r="5">
@@ -2333,10 +2333,10 @@
         <v>63.33</v>
       </c>
       <c r="BQ6" t="n">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="BR6" t="n">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="BS6" t="n">
         <v>0</v>
@@ -2345,19 +2345,19 @@
         <v>0</v>
       </c>
       <c r="BU6" t="n">
-        <v>555.7</v>
+        <v>276.9</v>
       </c>
       <c r="BV6" t="n">
-        <v>40.27</v>
+        <v>39.31</v>
       </c>
       <c r="BW6" t="n">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="BX6" t="n">
         <v>0</v>
       </c>
       <c r="BY6" t="n">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="BZ6" t="n">
         <v>142</v>
@@ -2375,7 +2375,7 @@
         <v>40</v>
       </c>
       <c r="CE6" t="n">
-        <v>2.26</v>
+        <v>2.21</v>
       </c>
       <c r="CF6" t="n">
         <v>16.42</v>
@@ -2384,25 +2384,25 @@
         <v>0.33</v>
       </c>
       <c r="CH6" t="n">
-        <v>6.75</v>
+        <v>6.67</v>
       </c>
       <c r="CI6" t="n">
-        <v>16.58</v>
+        <v>16.33</v>
       </c>
       <c r="CJ6" t="n">
-        <v>46.31</v>
+        <v>23.07</v>
       </c>
       <c r="CK6" t="n">
-        <v>3.36</v>
+        <v>3.28</v>
       </c>
       <c r="CL6" t="n">
-        <v>24.42</v>
+        <v>24.25</v>
       </c>
       <c r="CM6" t="n">
         <v>0</v>
       </c>
       <c r="CN6" t="n">
-        <v>1.75</v>
+        <v>1.58</v>
       </c>
       <c r="CO6" t="n">
         <v>11.83</v>
@@ -2634,10 +2634,10 @@
         <v>64.33</v>
       </c>
       <c r="BQ7" t="n">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="BR7" t="n">
-        <v>131</v>
+        <v>113</v>
       </c>
       <c r="BS7" t="n">
         <v>0</v>
@@ -2646,13 +2646,13 @@
         <v>0</v>
       </c>
       <c r="BU7" t="n">
-        <v>465.77</v>
+        <v>186.78</v>
       </c>
       <c r="BV7" t="n">
-        <v>37.38</v>
+        <v>34.42</v>
       </c>
       <c r="BW7" t="n">
-        <v>212</v>
+        <v>186</v>
       </c>
       <c r="BX7" t="n">
         <v>0</v>
@@ -2667,7 +2667,7 @@
         <v>2</v>
       </c>
       <c r="CB7" t="n">
-        <v>38</v>
+        <v>12</v>
       </c>
       <c r="CC7" t="n">
         <v>20</v>
@@ -2676,7 +2676,7 @@
         <v>18</v>
       </c>
       <c r="CE7" t="n">
-        <v>2.8</v>
+        <v>2.5</v>
       </c>
       <c r="CF7" t="n">
         <v>7.73</v>
@@ -2685,19 +2685,19 @@
         <v>0.36</v>
       </c>
       <c r="CH7" t="n">
-        <v>6.09</v>
+        <v>6</v>
       </c>
       <c r="CI7" t="n">
-        <v>11.91</v>
+        <v>10.27</v>
       </c>
       <c r="CJ7" t="n">
-        <v>42.34</v>
+        <v>16.98</v>
       </c>
       <c r="CK7" t="n">
-        <v>3.4</v>
+        <v>3.13</v>
       </c>
       <c r="CL7" t="n">
-        <v>19.27</v>
+        <v>16.91</v>
       </c>
       <c r="CM7" t="n">
         <v>0</v>
@@ -2712,7 +2712,7 @@
         <v>0.18</v>
       </c>
       <c r="CQ7" t="n">
-        <v>3.45</v>
+        <v>1.09</v>
       </c>
       <c r="CR7" t="n">
         <v>1.82</v>
@@ -2938,7 +2938,7 @@
         <v>100</v>
       </c>
       <c r="BR8" t="n">
-        <v>285</v>
+        <v>273</v>
       </c>
       <c r="BS8" t="n">
         <v>0</v>
@@ -2950,10 +2950,10 @@
         <v>218.33</v>
       </c>
       <c r="BV8" t="n">
-        <v>46.03</v>
+        <v>44.36</v>
       </c>
       <c r="BW8" t="n">
-        <v>462</v>
+        <v>348</v>
       </c>
       <c r="BX8" t="n">
         <v>0</v>
@@ -2965,10 +2965,10 @@
         <v>156</v>
       </c>
       <c r="CA8" t="n">
-        <v>60</v>
+        <v>4</v>
       </c>
       <c r="CB8" t="n">
-        <v>70</v>
+        <v>12</v>
       </c>
       <c r="CC8" t="n">
         <v>40</v>
@@ -2977,7 +2977,7 @@
         <v>90</v>
       </c>
       <c r="CE8" t="n">
-        <v>1.83</v>
+        <v>1.79</v>
       </c>
       <c r="CF8" t="n">
         <v>22.58</v>
@@ -2989,16 +2989,16 @@
         <v>8.33</v>
       </c>
       <c r="CI8" t="n">
-        <v>23.75</v>
+        <v>22.75</v>
       </c>
       <c r="CJ8" t="n">
         <v>18.19</v>
       </c>
       <c r="CK8" t="n">
-        <v>3.84</v>
+        <v>3.7</v>
       </c>
       <c r="CL8" t="n">
-        <v>38.5</v>
+        <v>29</v>
       </c>
       <c r="CM8" t="n">
         <v>0</v>
@@ -3010,10 +3010,10 @@
         <v>13</v>
       </c>
       <c r="CP8" t="n">
-        <v>5</v>
+        <v>0.33</v>
       </c>
       <c r="CQ8" t="n">
-        <v>5.83</v>
+        <v>1</v>
       </c>
       <c r="CR8" t="n">
         <v>3.33</v>

</xml_diff>

<commit_message>
Ahora los datos de analisis de salida tambien llevan el tiempo medio entre las interacciones como grab y realease
</commit_message>
<xml_diff>
--- a/data_analysis/db_env/app/results/global.xlsx
+++ b/data_analysis/db_env/app/results/global.xlsx
@@ -17,13 +17,16 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="1">
+  <fonts count="2">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
       <color theme="1"/>
       <sz val="11"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -34,7 +37,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -42,12 +45,21 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -413,14 +425,586 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A1"/>
+  <dimension ref="A1:BS2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1">
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>ID</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>GROUP</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>TD</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>GP_NUM</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>GP_NUM_START</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>GP_TIME</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>GP_TIME_START_TO_END</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>OI_NUM</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>OI_NUM_ACTOR_0</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>OI_NUM_ACTOR_1</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>OI_NUM_ACTOR_2</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>OI_NUM_ACTOR_3</t>
+        </is>
+      </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>OI_NUM_ACTOR_4</t>
+        </is>
+      </c>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
+          <t>OI_NUM_ACTOR_5</t>
+        </is>
+      </c>
+      <c r="P1" s="1" t="inlineStr">
+        <is>
+          <t>OI_NUM_ACTOR_6</t>
+        </is>
+      </c>
+      <c r="Q1" s="1" t="inlineStr">
+        <is>
+          <t>OI_NUM_ACTOR_7</t>
+        </is>
+      </c>
+      <c r="R1" s="1" t="inlineStr">
+        <is>
+          <t>OI_NUM_ACTOR_8</t>
+        </is>
+      </c>
+      <c r="S1" s="1" t="inlineStr">
+        <is>
+          <t>OI_NUM_ACTOR_9</t>
+        </is>
+      </c>
+      <c r="T1" s="1" t="inlineStr">
+        <is>
+          <t>OI_NUM_ACTOR_10</t>
+        </is>
+      </c>
+      <c r="U1" s="1" t="inlineStr">
+        <is>
+          <t>OI_NUM_ACTOR_11</t>
+        </is>
+      </c>
+      <c r="V1" s="1" t="inlineStr">
+        <is>
+          <t>OI_NUM_TYPE_DEFAULT</t>
+        </is>
+      </c>
+      <c r="W1" s="1" t="inlineStr">
+        <is>
+          <t>OI_NUM_TYPE_START_DETECTION</t>
+        </is>
+      </c>
+      <c r="X1" s="1" t="inlineStr">
+        <is>
+          <t>OI_NUM_TYPE_STOP_DETECTION</t>
+        </is>
+      </c>
+      <c r="Y1" s="1" t="inlineStr">
+        <is>
+          <t>OI_NUM_TYPE_GRAB</t>
+        </is>
+      </c>
+      <c r="Z1" s="1" t="inlineStr">
+        <is>
+          <t>OI_NUM_TYPE_RELEASE</t>
+        </is>
+      </c>
+      <c r="AA1" s="1" t="inlineStr">
+        <is>
+          <t>OI_TIME_INTER</t>
+        </is>
+      </c>
+      <c r="AB1" s="1" t="inlineStr">
+        <is>
+          <t>OI_TIME_CP_SS</t>
+        </is>
+      </c>
+      <c r="AC1" s="1" t="inlineStr">
+        <is>
+          <t>OI_TIME_CP_GR</t>
+        </is>
+      </c>
+      <c r="AD1" s="1" t="inlineStr">
+        <is>
+          <t>NPC_NUM</t>
+        </is>
+      </c>
+      <c r="AE1" s="1" t="inlineStr">
+        <is>
+          <t>NPC_NUM_ACTOR_0</t>
+        </is>
+      </c>
+      <c r="AF1" s="1" t="inlineStr">
+        <is>
+          <t>NPC_NUM_ACTOR_1</t>
+        </is>
+      </c>
+      <c r="AG1" s="1" t="inlineStr">
+        <is>
+          <t>NPC_NUM_ACTOR_2</t>
+        </is>
+      </c>
+      <c r="AH1" s="1" t="inlineStr">
+        <is>
+          <t>NPC_NUM_ACTOR_3</t>
+        </is>
+      </c>
+      <c r="AI1" s="1" t="inlineStr">
+        <is>
+          <t>NPC_NUM_ACTOR_4</t>
+        </is>
+      </c>
+      <c r="AJ1" s="1" t="inlineStr">
+        <is>
+          <t>NPC_NUM_ACTOR_5</t>
+        </is>
+      </c>
+      <c r="AK1" s="1" t="inlineStr">
+        <is>
+          <t>NPC_NUM_ACTOR_6</t>
+        </is>
+      </c>
+      <c r="AL1" s="1" t="inlineStr">
+        <is>
+          <t>NPC_NUM_ACTOR_7</t>
+        </is>
+      </c>
+      <c r="AM1" s="1" t="inlineStr">
+        <is>
+          <t>NPC_NUM_TYPE_DEFAULT</t>
+        </is>
+      </c>
+      <c r="AN1" s="1" t="inlineStr">
+        <is>
+          <t>NPC_NUM_TYPE_START_TALK_WITH_NPC</t>
+        </is>
+      </c>
+      <c r="AO1" s="1" t="inlineStr">
+        <is>
+          <t>NPC_NUM_TYPE_STOP_TALK_WITH_NPC</t>
+        </is>
+      </c>
+      <c r="AP1" s="1" t="inlineStr">
+        <is>
+          <t>NPC_TIME_INTER</t>
+        </is>
+      </c>
+      <c r="AQ1" s="1" t="inlineStr">
+        <is>
+          <t>MV_NUM_VR</t>
+        </is>
+      </c>
+      <c r="AR1" s="1" t="inlineStr">
+        <is>
+          <t>MV_NUM_RL</t>
+        </is>
+      </c>
+      <c r="AS1" s="1" t="inlineStr">
+        <is>
+          <t>MV_TIME_VR</t>
+        </is>
+      </c>
+      <c r="AT1" s="1" t="inlineStr">
+        <is>
+          <t>MV_TIME_RL</t>
+        </is>
+      </c>
+      <c r="AU1" s="1" t="inlineStr">
+        <is>
+          <t>MV_DIST_VR</t>
+        </is>
+      </c>
+      <c r="AV1" s="1" t="inlineStr">
+        <is>
+          <t>MV_DIST_RL</t>
+        </is>
+      </c>
+      <c r="AW1" s="1" t="inlineStr">
+        <is>
+          <t>UI_NUM</t>
+        </is>
+      </c>
+      <c r="AX1" s="1" t="inlineStr">
+        <is>
+          <t>UI_NUM_TYPE_DEFAULT</t>
+        </is>
+      </c>
+      <c r="AY1" s="1" t="inlineStr">
+        <is>
+          <t>UI_NUM_TYPE_IA_MOVE_LEFT</t>
+        </is>
+      </c>
+      <c r="AZ1" s="1" t="inlineStr">
+        <is>
+          <t>UI_NUM_TYPE_IA_MOVE_RIGHT</t>
+        </is>
+      </c>
+      <c r="BA1" s="1" t="inlineStr">
+        <is>
+          <t>UI_NUM_TYPE_IA_MENU_INTERACT_LEFT</t>
+        </is>
+      </c>
+      <c r="BB1" s="1" t="inlineStr">
+        <is>
+          <t>UI_NUM_TYPE_IA_MENU_INTERACT_RIGHT</t>
+        </is>
+      </c>
+      <c r="BC1" s="1" t="inlineStr">
+        <is>
+          <t>UI_NUM_TYPE_IA_GRAB_LEFT</t>
+        </is>
+      </c>
+      <c r="BD1" s="1" t="inlineStr">
+        <is>
+          <t>UI_NUM_TYPE_IA_GRAB_RIGHT</t>
+        </is>
+      </c>
+      <c r="BE1" s="1" t="inlineStr">
+        <is>
+          <t>UI_TIME</t>
+        </is>
+      </c>
+      <c r="BF1" s="1" t="inlineStr">
+        <is>
+          <t>OI_NUM_GP_STEPS</t>
+        </is>
+      </c>
+      <c r="BG1" s="1" t="inlineStr">
+        <is>
+          <t>NPC_NUM_GP_STEPS</t>
+        </is>
+      </c>
+      <c r="BH1" s="1" t="inlineStr">
+        <is>
+          <t>MV_NUM_VR_GP_STEPS</t>
+        </is>
+      </c>
+      <c r="BI1" s="1" t="inlineStr">
+        <is>
+          <t>MV_NUM_RL_GP_STEPS</t>
+        </is>
+      </c>
+      <c r="BJ1" s="1" t="inlineStr">
+        <is>
+          <t>MV_DIST_VR_GP_STEPS</t>
+        </is>
+      </c>
+      <c r="BK1" s="1" t="inlineStr">
+        <is>
+          <t>MV_DIST_RL_GP_STEPS</t>
+        </is>
+      </c>
+      <c r="BL1" s="1" t="inlineStr">
+        <is>
+          <t>UI_NUM_GP_STEPS</t>
+        </is>
+      </c>
+      <c r="BM1" s="1" t="inlineStr">
+        <is>
+          <t>UI_NUM_TYPE_DEFAULT_GP_STEPS</t>
+        </is>
+      </c>
+      <c r="BN1" s="1" t="inlineStr">
+        <is>
+          <t>UI_NUM_TYPE_IA_MOVE_LEFT_GP_STEPS</t>
+        </is>
+      </c>
+      <c r="BO1" s="1" t="inlineStr">
+        <is>
+          <t>UI_NUM_TYPE_IA_MOVE_RIGHT_GP_STEPS</t>
+        </is>
+      </c>
+      <c r="BP1" s="1" t="inlineStr">
+        <is>
+          <t>UI_NUM_TYPE_IA_MENU_INTERACT_LEFT_GP_STEPS</t>
+        </is>
+      </c>
+      <c r="BQ1" s="1" t="inlineStr">
+        <is>
+          <t>UI_NUM_TYPE_IA_MENU_INTERACT_RIGHT_GP_STEPS</t>
+        </is>
+      </c>
+      <c r="BR1" s="1" t="inlineStr">
+        <is>
+          <t>UI_NUM_TYPE_IA_GRAB_LEFT_GP_STEPS</t>
+        </is>
+      </c>
+      <c r="BS1" s="1" t="inlineStr">
+        <is>
+          <t>UI_NUM_TYPE_IA_GRAB_RIGHT_GP_STEPS</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>ale_0</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>TSV</t>
+        </is>
+      </c>
+      <c r="D2" t="n">
+        <v>626.4360001087189</v>
+      </c>
+      <c r="E2" t="n">
+        <v>10</v>
+      </c>
+      <c r="F2" t="n">
+        <v>11</v>
+      </c>
+      <c r="G2" t="n">
+        <v>49.22</v>
+      </c>
+      <c r="H2" t="n">
+        <v>48.28</v>
+      </c>
+      <c r="I2" t="n">
+        <v>91</v>
+      </c>
+      <c r="J2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K2" t="n">
+        <v>40</v>
+      </c>
+      <c r="L2" t="n">
+        <v>36</v>
+      </c>
+      <c r="M2" t="n">
+        <v>9</v>
+      </c>
+      <c r="N2" t="n">
+        <v>6</v>
+      </c>
+      <c r="O2" t="n">
+        <v>0</v>
+      </c>
+      <c r="P2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q2" t="n">
+        <v>0</v>
+      </c>
+      <c r="R2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S2" t="n">
+        <v>0</v>
+      </c>
+      <c r="T2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U2" t="n">
+        <v>0</v>
+      </c>
+      <c r="V2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W2" t="n">
+        <v>38</v>
+      </c>
+      <c r="X2" t="n">
+        <v>21</v>
+      </c>
+      <c r="Y2" t="n">
+        <v>16</v>
+      </c>
+      <c r="Z2" t="n">
+        <v>16</v>
+      </c>
+      <c r="AA2" t="n">
+        <v>3.22</v>
+      </c>
+      <c r="AB2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD2" t="n">
+        <v>4</v>
+      </c>
+      <c r="AE2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF2" t="n">
+        <v>4</v>
+      </c>
+      <c r="AG2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN2" t="n">
+        <v>2</v>
+      </c>
+      <c r="AO2" t="n">
+        <v>2</v>
+      </c>
+      <c r="AP2" t="n">
+        <v>67</v>
+      </c>
+      <c r="AQ2" t="n">
+        <v>100</v>
+      </c>
+      <c r="AR2" t="n">
+        <v>102</v>
+      </c>
+      <c r="AS2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AT2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU2" t="n">
+        <v>132.49</v>
+      </c>
+      <c r="AV2" t="n">
+        <v>15.85</v>
+      </c>
+      <c r="AW2" t="n">
+        <v>294</v>
+      </c>
+      <c r="AX2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AY2" t="n">
+        <v>4</v>
+      </c>
+      <c r="AZ2" t="n">
+        <v>214</v>
+      </c>
+      <c r="BA2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BB2" t="n">
+        <v>18</v>
+      </c>
+      <c r="BC2" t="n">
+        <v>22</v>
+      </c>
+      <c r="BD2" t="n">
+        <v>36</v>
+      </c>
+      <c r="BE2" t="n">
+        <v>1.22</v>
+      </c>
+      <c r="BF2" t="n">
+        <v>9.1</v>
+      </c>
+      <c r="BG2" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="BH2" t="n">
+        <v>10</v>
+      </c>
+      <c r="BI2" t="n">
+        <v>10.2</v>
+      </c>
+      <c r="BJ2" t="n">
+        <v>13.25</v>
+      </c>
+      <c r="BK2" t="n">
+        <v>1.58</v>
+      </c>
+      <c r="BL2" t="n">
+        <v>29.4</v>
+      </c>
+      <c r="BM2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BN2" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="BO2" t="n">
+        <v>21.4</v>
+      </c>
+      <c r="BP2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BQ2" t="n">
+        <v>1.8</v>
+      </c>
+      <c r="BR2" t="n">
+        <v>2.2</v>
+      </c>
+      <c r="BS2" t="n">
+        <v>3.6</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Arreglados los errores del analisis. Ahora estoy intentando que todos los usuarios tengan el mismo ID de usuario
</commit_message>
<xml_diff>
--- a/data_analysis/db_env/app/results/global.xlsx
+++ b/data_analysis/db_env/app/results/global.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:BS2"/>
+  <dimension ref="A1:BS9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -791,7 +791,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>ale_0</t>
+          <t>AA_0</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -800,37 +800,37 @@
         </is>
       </c>
       <c r="D2" t="n">
-        <v>626.4360001087189</v>
+        <v>750.91</v>
       </c>
       <c r="E2" t="n">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="F2" t="n">
         <v>11</v>
       </c>
       <c r="G2" t="n">
-        <v>49.22</v>
+        <v>70.91</v>
       </c>
       <c r="H2" t="n">
-        <v>48.28</v>
+        <v>70.19</v>
       </c>
       <c r="I2" t="n">
-        <v>91</v>
+        <v>120</v>
       </c>
       <c r="J2" t="n">
         <v>0</v>
       </c>
       <c r="K2" t="n">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="L2" t="n">
-        <v>36</v>
+        <v>48</v>
       </c>
       <c r="M2" t="n">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="N2" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="O2" t="n">
         <v>0</v>
@@ -857,25 +857,25 @@
         <v>0</v>
       </c>
       <c r="W2" t="n">
-        <v>38</v>
+        <v>45</v>
       </c>
       <c r="X2" t="n">
-        <v>21</v>
+        <v>45</v>
       </c>
       <c r="Y2" t="n">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="Z2" t="n">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="AA2" t="n">
-        <v>3.22</v>
+        <v>4.66</v>
       </c>
       <c r="AB2" t="n">
-        <v>0</v>
+        <v>0.53</v>
       </c>
       <c r="AC2" t="n">
-        <v>0</v>
+        <v>-4.46</v>
       </c>
       <c r="AD2" t="n">
         <v>4</v>
@@ -914,13 +914,13 @@
         <v>2</v>
       </c>
       <c r="AP2" t="n">
-        <v>67</v>
+        <v>138.67</v>
       </c>
       <c r="AQ2" t="n">
-        <v>100</v>
+        <v>69</v>
       </c>
       <c r="AR2" t="n">
-        <v>102</v>
+        <v>238</v>
       </c>
       <c r="AS2" t="n">
         <v>0</v>
@@ -929,79 +929,1612 @@
         <v>0</v>
       </c>
       <c r="AU2" t="n">
-        <v>132.49</v>
+        <v>189.92</v>
       </c>
       <c r="AV2" t="n">
-        <v>15.85</v>
+        <v>42.13</v>
       </c>
       <c r="AW2" t="n">
-        <v>294</v>
+        <v>216</v>
       </c>
       <c r="AX2" t="n">
         <v>0</v>
       </c>
       <c r="AY2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AZ2" t="n">
+        <v>138</v>
+      </c>
+      <c r="BA2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BB2" t="n">
+        <v>24</v>
+      </c>
+      <c r="BC2" t="n">
+        <v>8</v>
+      </c>
+      <c r="BD2" t="n">
+        <v>46</v>
+      </c>
+      <c r="BE2" t="n">
+        <v>3.16</v>
+      </c>
+      <c r="BF2" t="n">
+        <v>10</v>
+      </c>
+      <c r="BG2" t="n">
+        <v>0.33</v>
+      </c>
+      <c r="BH2" t="n">
+        <v>5.75</v>
+      </c>
+      <c r="BI2" t="n">
+        <v>19.83</v>
+      </c>
+      <c r="BJ2" t="n">
+        <v>15.83</v>
+      </c>
+      <c r="BK2" t="n">
+        <v>3.51</v>
+      </c>
+      <c r="BL2" t="n">
+        <v>18</v>
+      </c>
+      <c r="BM2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BN2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BO2" t="n">
+        <v>11.5</v>
+      </c>
+      <c r="BP2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BQ2" t="n">
+        <v>2</v>
+      </c>
+      <c r="BR2" t="n">
+        <v>0.67</v>
+      </c>
+      <c r="BS2" t="n">
+        <v>3.83</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>AA_1</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>TSV</t>
+        </is>
+      </c>
+      <c r="D3" t="n">
+        <v>1238.63</v>
+      </c>
+      <c r="E3" t="n">
+        <v>17</v>
+      </c>
+      <c r="F3" t="n">
+        <v>7</v>
+      </c>
+      <c r="G3" t="n">
+        <v>78.25</v>
+      </c>
+      <c r="H3" t="n">
+        <v>72.72</v>
+      </c>
+      <c r="I3" t="n">
+        <v>96</v>
+      </c>
+      <c r="J3" t="n">
+        <v>0</v>
+      </c>
+      <c r="K3" t="n">
+        <v>0</v>
+      </c>
+      <c r="L3" t="n">
+        <v>62</v>
+      </c>
+      <c r="M3" t="n">
+        <v>3</v>
+      </c>
+      <c r="N3" t="n">
+        <v>3</v>
+      </c>
+      <c r="O3" t="n">
+        <v>19</v>
+      </c>
+      <c r="P3" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q3" t="n">
+        <v>0</v>
+      </c>
+      <c r="R3" t="n">
+        <v>0</v>
+      </c>
+      <c r="S3" t="n">
+        <v>0</v>
+      </c>
+      <c r="T3" t="n">
+        <v>0</v>
+      </c>
+      <c r="U3" t="n">
+        <v>9</v>
+      </c>
+      <c r="V3" t="n">
+        <v>0</v>
+      </c>
+      <c r="W3" t="n">
+        <v>26</v>
+      </c>
+      <c r="X3" t="n">
+        <v>34</v>
+      </c>
+      <c r="Y3" t="n">
+        <v>18</v>
+      </c>
+      <c r="Z3" t="n">
+        <v>18</v>
+      </c>
+      <c r="AA3" t="n">
+        <v>10.83</v>
+      </c>
+      <c r="AB3" t="n">
+        <v>-63.48</v>
+      </c>
+      <c r="AC3" t="n">
+        <v>29.28</v>
+      </c>
+      <c r="AD3" t="n">
+        <v>6</v>
+      </c>
+      <c r="AE3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG3" t="n">
+        <v>2</v>
+      </c>
+      <c r="AH3" t="n">
         <v>4</v>
       </c>
-      <c r="AZ2" t="n">
-        <v>214</v>
-      </c>
-      <c r="BA2" t="n">
-        <v>0</v>
-      </c>
-      <c r="BB2" t="n">
+      <c r="AI3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN3" t="n">
+        <v>3</v>
+      </c>
+      <c r="AO3" t="n">
+        <v>3</v>
+      </c>
+      <c r="AP3" t="n">
+        <v>23.6</v>
+      </c>
+      <c r="AQ3" t="n">
+        <v>129</v>
+      </c>
+      <c r="AR3" t="n">
+        <v>217</v>
+      </c>
+      <c r="AS3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AT3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU3" t="n">
+        <v>402.72</v>
+      </c>
+      <c r="AV3" t="n">
+        <v>37.5</v>
+      </c>
+      <c r="AW3" t="n">
+        <v>706</v>
+      </c>
+      <c r="AX3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AY3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AZ3" t="n">
+        <v>262</v>
+      </c>
+      <c r="BA3" t="n">
+        <v>106</v>
+      </c>
+      <c r="BB3" t="n">
+        <v>258</v>
+      </c>
+      <c r="BC3" t="n">
         <v>18</v>
       </c>
-      <c r="BC2" t="n">
+      <c r="BD3" t="n">
+        <v>44</v>
+      </c>
+      <c r="BE3" t="n">
+        <v>1.66</v>
+      </c>
+      <c r="BF3" t="n">
+        <v>5.65</v>
+      </c>
+      <c r="BG3" t="n">
+        <v>0.35</v>
+      </c>
+      <c r="BH3" t="n">
+        <v>7.59</v>
+      </c>
+      <c r="BI3" t="n">
+        <v>12.76</v>
+      </c>
+      <c r="BJ3" t="n">
+        <v>23.69</v>
+      </c>
+      <c r="BK3" t="n">
+        <v>2.21</v>
+      </c>
+      <c r="BL3" t="n">
+        <v>41.53</v>
+      </c>
+      <c r="BM3" t="n">
+        <v>0</v>
+      </c>
+      <c r="BN3" t="n">
+        <v>0</v>
+      </c>
+      <c r="BO3" t="n">
+        <v>15.41</v>
+      </c>
+      <c r="BP3" t="n">
+        <v>6.24</v>
+      </c>
+      <c r="BQ3" t="n">
+        <v>15.18</v>
+      </c>
+      <c r="BR3" t="n">
+        <v>1.06</v>
+      </c>
+      <c r="BS3" t="n">
+        <v>2.59</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>AB_0</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>TS</t>
+        </is>
+      </c>
+      <c r="D4" t="n">
+        <v>380.58</v>
+      </c>
+      <c r="E4" t="n">
+        <v>10</v>
+      </c>
+      <c r="F4" t="n">
+        <v>10</v>
+      </c>
+      <c r="G4" t="n">
+        <v>42.33</v>
+      </c>
+      <c r="H4" t="n">
+        <v>41.36</v>
+      </c>
+      <c r="I4" t="n">
+        <v>126</v>
+      </c>
+      <c r="J4" t="n">
+        <v>0</v>
+      </c>
+      <c r="K4" t="n">
+        <v>64</v>
+      </c>
+      <c r="L4" t="n">
+        <v>36</v>
+      </c>
+      <c r="M4" t="n">
+        <v>16</v>
+      </c>
+      <c r="N4" t="n">
+        <v>10</v>
+      </c>
+      <c r="O4" t="n">
+        <v>0</v>
+      </c>
+      <c r="P4" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q4" t="n">
+        <v>0</v>
+      </c>
+      <c r="R4" t="n">
+        <v>0</v>
+      </c>
+      <c r="S4" t="n">
+        <v>0</v>
+      </c>
+      <c r="T4" t="n">
+        <v>0</v>
+      </c>
+      <c r="U4" t="n">
+        <v>0</v>
+      </c>
+      <c r="V4" t="n">
+        <v>0</v>
+      </c>
+      <c r="W4" t="n">
+        <v>40</v>
+      </c>
+      <c r="X4" t="n">
+        <v>40</v>
+      </c>
+      <c r="Y4" t="n">
+        <v>23</v>
+      </c>
+      <c r="Z4" t="n">
+        <v>23</v>
+      </c>
+      <c r="AA4" t="n">
+        <v>2.17</v>
+      </c>
+      <c r="AB4" t="n">
+        <v>0.16</v>
+      </c>
+      <c r="AC4" t="n">
+        <v>0.44</v>
+      </c>
+      <c r="AD4" t="n">
+        <v>4</v>
+      </c>
+      <c r="AE4" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF4" t="n">
+        <v>4</v>
+      </c>
+      <c r="AG4" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH4" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI4" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ4" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK4" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL4" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM4" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN4" t="n">
+        <v>2</v>
+      </c>
+      <c r="AO4" t="n">
+        <v>2</v>
+      </c>
+      <c r="AP4" t="n">
+        <v>59</v>
+      </c>
+      <c r="AQ4" t="n">
+        <v>62</v>
+      </c>
+      <c r="AR4" t="n">
+        <v>149</v>
+      </c>
+      <c r="AS4" t="n">
+        <v>0</v>
+      </c>
+      <c r="AT4" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU4" t="n">
+        <v>163.56</v>
+      </c>
+      <c r="AV4" t="n">
+        <v>25.63</v>
+      </c>
+      <c r="AW4" t="n">
+        <v>564</v>
+      </c>
+      <c r="AX4" t="n">
+        <v>0</v>
+      </c>
+      <c r="AY4" t="n">
+        <v>0</v>
+      </c>
+      <c r="AZ4" t="n">
+        <v>124</v>
+      </c>
+      <c r="BA4" t="n">
+        <v>0</v>
+      </c>
+      <c r="BB4" t="n">
+        <v>34</v>
+      </c>
+      <c r="BC4" t="n">
+        <v>30</v>
+      </c>
+      <c r="BD4" t="n">
+        <v>376</v>
+      </c>
+      <c r="BE4" t="n">
+        <v>0.68</v>
+      </c>
+      <c r="BF4" t="n">
+        <v>12.6</v>
+      </c>
+      <c r="BG4" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="BH4" t="n">
+        <v>6.2</v>
+      </c>
+      <c r="BI4" t="n">
+        <v>14.9</v>
+      </c>
+      <c r="BJ4" t="n">
+        <v>16.36</v>
+      </c>
+      <c r="BK4" t="n">
+        <v>2.56</v>
+      </c>
+      <c r="BL4" t="n">
+        <v>56.4</v>
+      </c>
+      <c r="BM4" t="n">
+        <v>0</v>
+      </c>
+      <c r="BN4" t="n">
+        <v>0</v>
+      </c>
+      <c r="BO4" t="n">
+        <v>12.4</v>
+      </c>
+      <c r="BP4" t="n">
+        <v>0</v>
+      </c>
+      <c r="BQ4" t="n">
+        <v>3.4</v>
+      </c>
+      <c r="BR4" t="n">
+        <v>3</v>
+      </c>
+      <c r="BS4" t="n">
+        <v>37.6</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>AB_1</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>TS</t>
+        </is>
+      </c>
+      <c r="D5" t="n">
+        <v>951.95</v>
+      </c>
+      <c r="E5" t="n">
+        <v>18</v>
+      </c>
+      <c r="F5" t="n">
+        <v>7</v>
+      </c>
+      <c r="G5" t="n">
+        <v>56.94</v>
+      </c>
+      <c r="H5" t="n">
+        <v>38.75</v>
+      </c>
+      <c r="I5" t="n">
+        <v>113</v>
+      </c>
+      <c r="J5" t="n">
+        <v>0</v>
+      </c>
+      <c r="K5" t="n">
+        <v>0</v>
+      </c>
+      <c r="L5" t="n">
+        <v>16</v>
+      </c>
+      <c r="M5" t="n">
+        <v>27</v>
+      </c>
+      <c r="N5" t="n">
+        <v>15</v>
+      </c>
+      <c r="O5" t="n">
+        <v>36</v>
+      </c>
+      <c r="P5" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q5" t="n">
+        <v>0</v>
+      </c>
+      <c r="R5" t="n">
+        <v>0</v>
+      </c>
+      <c r="S5" t="n">
+        <v>0</v>
+      </c>
+      <c r="T5" t="n">
+        <v>0</v>
+      </c>
+      <c r="U5" t="n">
+        <v>19</v>
+      </c>
+      <c r="V5" t="n">
+        <v>0</v>
+      </c>
+      <c r="W5" t="n">
+        <v>34</v>
+      </c>
+      <c r="X5" t="n">
+        <v>40</v>
+      </c>
+      <c r="Y5" t="n">
         <v>22</v>
       </c>
-      <c r="BD2" t="n">
+      <c r="Z5" t="n">
+        <v>17</v>
+      </c>
+      <c r="AA5" t="n">
+        <v>7.83</v>
+      </c>
+      <c r="AB5" t="n">
+        <v>-94.2</v>
+      </c>
+      <c r="AC5" t="n">
+        <v>59.5</v>
+      </c>
+      <c r="AD5" t="n">
+        <v>10</v>
+      </c>
+      <c r="AE5" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF5" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG5" t="n">
+        <v>4</v>
+      </c>
+      <c r="AH5" t="n">
+        <v>6</v>
+      </c>
+      <c r="AI5" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ5" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK5" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL5" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM5" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN5" t="n">
+        <v>5</v>
+      </c>
+      <c r="AO5" t="n">
+        <v>5</v>
+      </c>
+      <c r="AP5" t="n">
+        <v>44</v>
+      </c>
+      <c r="AQ5" t="n">
+        <v>308</v>
+      </c>
+      <c r="AR5" t="n">
+        <v>200</v>
+      </c>
+      <c r="AS5" t="n">
+        <v>0</v>
+      </c>
+      <c r="AT5" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU5" t="n">
+        <v>876.74</v>
+      </c>
+      <c r="AV5" t="n">
+        <v>32.14</v>
+      </c>
+      <c r="AW5" t="n">
+        <v>985</v>
+      </c>
+      <c r="AX5" t="n">
+        <v>0</v>
+      </c>
+      <c r="AY5" t="n">
+        <v>50</v>
+      </c>
+      <c r="AZ5" t="n">
+        <v>568</v>
+      </c>
+      <c r="BA5" t="n">
+        <v>66</v>
+      </c>
+      <c r="BB5" t="n">
+        <v>136</v>
+      </c>
+      <c r="BC5" t="n">
+        <v>54</v>
+      </c>
+      <c r="BD5" t="n">
+        <v>95</v>
+      </c>
+      <c r="BE5" t="n">
+        <v>0.97</v>
+      </c>
+      <c r="BF5" t="n">
+        <v>6.28</v>
+      </c>
+      <c r="BG5" t="n">
+        <v>0.5600000000000001</v>
+      </c>
+      <c r="BH5" t="n">
+        <v>17.11</v>
+      </c>
+      <c r="BI5" t="n">
+        <v>11.11</v>
+      </c>
+      <c r="BJ5" t="n">
+        <v>48.71</v>
+      </c>
+      <c r="BK5" t="n">
+        <v>1.79</v>
+      </c>
+      <c r="BL5" t="n">
+        <v>54.72</v>
+      </c>
+      <c r="BM5" t="n">
+        <v>0</v>
+      </c>
+      <c r="BN5" t="n">
+        <v>2.78</v>
+      </c>
+      <c r="BO5" t="n">
+        <v>31.56</v>
+      </c>
+      <c r="BP5" t="n">
+        <v>3.67</v>
+      </c>
+      <c r="BQ5" t="n">
+        <v>7.56</v>
+      </c>
+      <c r="BR5" t="n">
+        <v>3</v>
+      </c>
+      <c r="BS5" t="n">
+        <v>5.28</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>AC_0</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>TSV</t>
+        </is>
+      </c>
+      <c r="D6" t="n">
+        <v>380.73</v>
+      </c>
+      <c r="E6" t="n">
+        <v>10</v>
+      </c>
+      <c r="F6" t="n">
+        <v>10</v>
+      </c>
+      <c r="G6" t="n">
+        <v>42.22</v>
+      </c>
+      <c r="H6" t="n">
+        <v>41.32</v>
+      </c>
+      <c r="I6" t="n">
+        <v>88</v>
+      </c>
+      <c r="J6" t="n">
+        <v>0</v>
+      </c>
+      <c r="K6" t="n">
+        <v>38</v>
+      </c>
+      <c r="L6" t="n">
+        <v>24</v>
+      </c>
+      <c r="M6" t="n">
+        <v>18</v>
+      </c>
+      <c r="N6" t="n">
+        <v>8</v>
+      </c>
+      <c r="O6" t="n">
+        <v>0</v>
+      </c>
+      <c r="P6" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q6" t="n">
+        <v>0</v>
+      </c>
+      <c r="R6" t="n">
+        <v>0</v>
+      </c>
+      <c r="S6" t="n">
+        <v>0</v>
+      </c>
+      <c r="T6" t="n">
+        <v>0</v>
+      </c>
+      <c r="U6" t="n">
+        <v>0</v>
+      </c>
+      <c r="V6" t="n">
+        <v>0</v>
+      </c>
+      <c r="W6" t="n">
+        <v>26</v>
+      </c>
+      <c r="X6" t="n">
+        <v>26</v>
+      </c>
+      <c r="Y6" t="n">
+        <v>18</v>
+      </c>
+      <c r="Z6" t="n">
+        <v>18</v>
+      </c>
+      <c r="AA6" t="n">
+        <v>2.95</v>
+      </c>
+      <c r="AB6" t="n">
+        <v>0.27</v>
+      </c>
+      <c r="AC6" t="n">
+        <v>3.94</v>
+      </c>
+      <c r="AD6" t="n">
+        <v>6</v>
+      </c>
+      <c r="AE6" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF6" t="n">
+        <v>6</v>
+      </c>
+      <c r="AG6" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH6" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI6" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ6" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK6" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL6" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM6" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN6" t="n">
+        <v>3</v>
+      </c>
+      <c r="AO6" t="n">
+        <v>3</v>
+      </c>
+      <c r="AP6" t="n">
+        <v>31.8</v>
+      </c>
+      <c r="AQ6" t="n">
+        <v>53</v>
+      </c>
+      <c r="AR6" t="n">
+        <v>203</v>
+      </c>
+      <c r="AS6" t="n">
+        <v>0</v>
+      </c>
+      <c r="AT6" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU6" t="n">
+        <v>191.1</v>
+      </c>
+      <c r="AV6" t="n">
+        <v>39.19</v>
+      </c>
+      <c r="AW6" t="n">
+        <v>195</v>
+      </c>
+      <c r="AX6" t="n">
+        <v>0</v>
+      </c>
+      <c r="AY6" t="n">
+        <v>90</v>
+      </c>
+      <c r="AZ6" t="n">
+        <v>17</v>
+      </c>
+      <c r="BA6" t="n">
+        <v>4</v>
+      </c>
+      <c r="BB6" t="n">
+        <v>42</v>
+      </c>
+      <c r="BC6" t="n">
+        <v>6</v>
+      </c>
+      <c r="BD6" t="n">
         <v>36</v>
       </c>
-      <c r="BE2" t="n">
-        <v>1.22</v>
-      </c>
-      <c r="BF2" t="n">
-        <v>9.1</v>
-      </c>
-      <c r="BG2" t="n">
+      <c r="BE6" t="n">
+        <v>1.85</v>
+      </c>
+      <c r="BF6" t="n">
+        <v>8.800000000000001</v>
+      </c>
+      <c r="BG6" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="BH6" t="n">
+        <v>5.3</v>
+      </c>
+      <c r="BI6" t="n">
+        <v>20.3</v>
+      </c>
+      <c r="BJ6" t="n">
+        <v>19.11</v>
+      </c>
+      <c r="BK6" t="n">
+        <v>3.92</v>
+      </c>
+      <c r="BL6" t="n">
+        <v>19.5</v>
+      </c>
+      <c r="BM6" t="n">
+        <v>0</v>
+      </c>
+      <c r="BN6" t="n">
+        <v>9</v>
+      </c>
+      <c r="BO6" t="n">
+        <v>1.7</v>
+      </c>
+      <c r="BP6" t="n">
         <v>0.4</v>
       </c>
-      <c r="BH2" t="n">
+      <c r="BQ6" t="n">
+        <v>4.2</v>
+      </c>
+      <c r="BR6" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="BS6" t="n">
+        <v>3.6</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>AC_1</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>TSV</t>
+        </is>
+      </c>
+      <c r="D7" t="n">
+        <v>712.22</v>
+      </c>
+      <c r="E7" t="n">
+        <v>15</v>
+      </c>
+      <c r="F7" t="n">
+        <v>7</v>
+      </c>
+      <c r="G7" t="n">
+        <v>50.79</v>
+      </c>
+      <c r="H7" t="n">
+        <v>46.34</v>
+      </c>
+      <c r="I7" t="n">
+        <v>68</v>
+      </c>
+      <c r="J7" t="n">
+        <v>0</v>
+      </c>
+      <c r="K7" t="n">
+        <v>0</v>
+      </c>
+      <c r="L7" t="n">
+        <v>8</v>
+      </c>
+      <c r="M7" t="n">
+        <v>25</v>
+      </c>
+      <c r="N7" t="n">
+        <v>19</v>
+      </c>
+      <c r="O7" t="n">
+        <v>14</v>
+      </c>
+      <c r="P7" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q7" t="n">
+        <v>0</v>
+      </c>
+      <c r="R7" t="n">
+        <v>0</v>
+      </c>
+      <c r="S7" t="n">
+        <v>0</v>
+      </c>
+      <c r="T7" t="n">
+        <v>0</v>
+      </c>
+      <c r="U7" t="n">
+        <v>2</v>
+      </c>
+      <c r="V7" t="n">
+        <v>0</v>
+      </c>
+      <c r="W7" t="n">
+        <v>16</v>
+      </c>
+      <c r="X7" t="n">
+        <v>21</v>
+      </c>
+      <c r="Y7" t="n">
+        <v>16</v>
+      </c>
+      <c r="Z7" t="n">
+        <v>15</v>
+      </c>
+      <c r="AA7" t="n">
+        <v>8.69</v>
+      </c>
+      <c r="AB7" t="n">
+        <v>-61.18</v>
+      </c>
+      <c r="AC7" t="n">
+        <v>27.05</v>
+      </c>
+      <c r="AD7" t="n">
+        <v>6</v>
+      </c>
+      <c r="AE7" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF7" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG7" t="n">
+        <v>2</v>
+      </c>
+      <c r="AH7" t="n">
+        <v>4</v>
+      </c>
+      <c r="AI7" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ7" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK7" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL7" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM7" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN7" t="n">
+        <v>3</v>
+      </c>
+      <c r="AO7" t="n">
+        <v>3</v>
+      </c>
+      <c r="AP7" t="n">
+        <v>19.6</v>
+      </c>
+      <c r="AQ7" t="n">
+        <v>101</v>
+      </c>
+      <c r="AR7" t="n">
+        <v>227</v>
+      </c>
+      <c r="AS7" t="n">
+        <v>0</v>
+      </c>
+      <c r="AT7" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU7" t="n">
+        <v>336.71</v>
+      </c>
+      <c r="AV7" t="n">
+        <v>38.03</v>
+      </c>
+      <c r="AW7" t="n">
+        <v>372</v>
+      </c>
+      <c r="AX7" t="n">
+        <v>0</v>
+      </c>
+      <c r="AY7" t="n">
+        <v>184</v>
+      </c>
+      <c r="AZ7" t="n">
+        <v>26</v>
+      </c>
+      <c r="BA7" t="n">
+        <v>16</v>
+      </c>
+      <c r="BB7" t="n">
+        <v>88</v>
+      </c>
+      <c r="BC7" t="n">
+        <v>6</v>
+      </c>
+      <c r="BD7" t="n">
+        <v>30</v>
+      </c>
+      <c r="BE7" t="n">
+        <v>1.91</v>
+      </c>
+      <c r="BF7" t="n">
+        <v>4.53</v>
+      </c>
+      <c r="BG7" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="BH7" t="n">
+        <v>6.73</v>
+      </c>
+      <c r="BI7" t="n">
+        <v>15.13</v>
+      </c>
+      <c r="BJ7" t="n">
+        <v>22.45</v>
+      </c>
+      <c r="BK7" t="n">
+        <v>2.54</v>
+      </c>
+      <c r="BL7" t="n">
+        <v>24.8</v>
+      </c>
+      <c r="BM7" t="n">
+        <v>0</v>
+      </c>
+      <c r="BN7" t="n">
+        <v>12.27</v>
+      </c>
+      <c r="BO7" t="n">
+        <v>1.73</v>
+      </c>
+      <c r="BP7" t="n">
+        <v>1.07</v>
+      </c>
+      <c r="BQ7" t="n">
+        <v>5.87</v>
+      </c>
+      <c r="BR7" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="BS7" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>AD_0</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>TS</t>
+        </is>
+      </c>
+      <c r="D8" t="n">
+        <v>579</v>
+      </c>
+      <c r="E8" t="n">
+        <v>12</v>
+      </c>
+      <c r="F8" t="n">
+        <v>11</v>
+      </c>
+      <c r="G8" t="n">
+        <v>55.36</v>
+      </c>
+      <c r="H8" t="n">
+        <v>54.55</v>
+      </c>
+      <c r="I8" t="n">
+        <v>90</v>
+      </c>
+      <c r="J8" t="n">
+        <v>0</v>
+      </c>
+      <c r="K8" t="n">
+        <v>34</v>
+      </c>
+      <c r="L8" t="n">
+        <v>28</v>
+      </c>
+      <c r="M8" t="n">
+        <v>18</v>
+      </c>
+      <c r="N8" t="n">
         <v>10</v>
       </c>
-      <c r="BI2" t="n">
-        <v>10.2</v>
-      </c>
-      <c r="BJ2" t="n">
-        <v>13.25</v>
-      </c>
-      <c r="BK2" t="n">
-        <v>1.58</v>
-      </c>
-      <c r="BL2" t="n">
-        <v>29.4</v>
-      </c>
-      <c r="BM2" t="n">
-        <v>0</v>
-      </c>
-      <c r="BN2" t="n">
+      <c r="O8" t="n">
+        <v>0</v>
+      </c>
+      <c r="P8" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q8" t="n">
+        <v>0</v>
+      </c>
+      <c r="R8" t="n">
+        <v>0</v>
+      </c>
+      <c r="S8" t="n">
+        <v>0</v>
+      </c>
+      <c r="T8" t="n">
+        <v>0</v>
+      </c>
+      <c r="U8" t="n">
+        <v>0</v>
+      </c>
+      <c r="V8" t="n">
+        <v>0</v>
+      </c>
+      <c r="W8" t="n">
+        <v>31</v>
+      </c>
+      <c r="X8" t="n">
+        <v>31</v>
+      </c>
+      <c r="Y8" t="n">
+        <v>14</v>
+      </c>
+      <c r="Z8" t="n">
+        <v>14</v>
+      </c>
+      <c r="AA8" t="n">
+        <v>4.13</v>
+      </c>
+      <c r="AB8" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="AC8" t="n">
+        <v>8.67</v>
+      </c>
+      <c r="AD8" t="n">
+        <v>4</v>
+      </c>
+      <c r="AE8" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF8" t="n">
+        <v>4</v>
+      </c>
+      <c r="AG8" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH8" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI8" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ8" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK8" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL8" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM8" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN8" t="n">
+        <v>2</v>
+      </c>
+      <c r="AO8" t="n">
+        <v>2</v>
+      </c>
+      <c r="AP8" t="n">
+        <v>85</v>
+      </c>
+      <c r="AQ8" t="n">
+        <v>44</v>
+      </c>
+      <c r="AR8" t="n">
+        <v>234</v>
+      </c>
+      <c r="AS8" t="n">
+        <v>0</v>
+      </c>
+      <c r="AT8" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU8" t="n">
+        <v>172.15</v>
+      </c>
+      <c r="AV8" t="n">
+        <v>39.04</v>
+      </c>
+      <c r="AW8" t="n">
+        <v>150</v>
+      </c>
+      <c r="AX8" t="n">
+        <v>0</v>
+      </c>
+      <c r="AY8" t="n">
+        <v>2</v>
+      </c>
+      <c r="AZ8" t="n">
+        <v>86</v>
+      </c>
+      <c r="BA8" t="n">
+        <v>4</v>
+      </c>
+      <c r="BB8" t="n">
+        <v>14</v>
+      </c>
+      <c r="BC8" t="n">
+        <v>18</v>
+      </c>
+      <c r="BD8" t="n">
+        <v>26</v>
+      </c>
+      <c r="BE8" t="n">
+        <v>3.63</v>
+      </c>
+      <c r="BF8" t="n">
+        <v>7.5</v>
+      </c>
+      <c r="BG8" t="n">
+        <v>0.33</v>
+      </c>
+      <c r="BH8" t="n">
+        <v>3.67</v>
+      </c>
+      <c r="BI8" t="n">
+        <v>19.5</v>
+      </c>
+      <c r="BJ8" t="n">
+        <v>14.35</v>
+      </c>
+      <c r="BK8" t="n">
+        <v>3.25</v>
+      </c>
+      <c r="BL8" t="n">
+        <v>12.5</v>
+      </c>
+      <c r="BM8" t="n">
+        <v>0</v>
+      </c>
+      <c r="BN8" t="n">
+        <v>0.17</v>
+      </c>
+      <c r="BO8" t="n">
+        <v>7.17</v>
+      </c>
+      <c r="BP8" t="n">
+        <v>0.33</v>
+      </c>
+      <c r="BQ8" t="n">
+        <v>1.17</v>
+      </c>
+      <c r="BR8" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="BS8" t="n">
+        <v>2.17</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>AD_1</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>TS</t>
+        </is>
+      </c>
+      <c r="D9" t="n">
+        <v>783.59</v>
+      </c>
+      <c r="E9" t="n">
+        <v>15</v>
+      </c>
+      <c r="F9" t="n">
+        <v>6</v>
+      </c>
+      <c r="G9" t="n">
+        <v>57.21</v>
+      </c>
+      <c r="H9" t="n">
+        <v>45.79</v>
+      </c>
+      <c r="I9" t="n">
+        <v>61</v>
+      </c>
+      <c r="J9" t="n">
+        <v>0</v>
+      </c>
+      <c r="K9" t="n">
+        <v>0</v>
+      </c>
+      <c r="L9" t="n">
+        <v>6</v>
+      </c>
+      <c r="M9" t="n">
+        <v>15</v>
+      </c>
+      <c r="N9" t="n">
+        <v>17</v>
+      </c>
+      <c r="O9" t="n">
+        <v>9</v>
+      </c>
+      <c r="P9" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q9" t="n">
+        <v>0</v>
+      </c>
+      <c r="R9" t="n">
+        <v>0</v>
+      </c>
+      <c r="S9" t="n">
+        <v>0</v>
+      </c>
+      <c r="T9" t="n">
+        <v>0</v>
+      </c>
+      <c r="U9" t="n">
+        <v>14</v>
+      </c>
+      <c r="V9" t="n">
+        <v>0</v>
+      </c>
+      <c r="W9" t="n">
+        <v>15</v>
+      </c>
+      <c r="X9" t="n">
+        <v>20</v>
+      </c>
+      <c r="Y9" t="n">
+        <v>13</v>
+      </c>
+      <c r="Z9" t="n">
+        <v>13</v>
+      </c>
+      <c r="AA9" t="n">
+        <v>10.48</v>
+      </c>
+      <c r="AB9" t="n">
+        <v>-106.33</v>
+      </c>
+      <c r="AC9" t="n">
+        <v>85.83</v>
+      </c>
+      <c r="AD9" t="n">
+        <v>6</v>
+      </c>
+      <c r="AE9" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF9" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG9" t="n">
+        <v>2</v>
+      </c>
+      <c r="AH9" t="n">
+        <v>4</v>
+      </c>
+      <c r="AI9" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ9" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK9" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL9" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM9" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN9" t="n">
+        <v>3</v>
+      </c>
+      <c r="AO9" t="n">
+        <v>3</v>
+      </c>
+      <c r="AP9" t="n">
+        <v>26.8</v>
+      </c>
+      <c r="AQ9" t="n">
+        <v>116</v>
+      </c>
+      <c r="AR9" t="n">
+        <v>293</v>
+      </c>
+      <c r="AS9" t="n">
+        <v>0</v>
+      </c>
+      <c r="AT9" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU9" t="n">
+        <v>315.86</v>
+      </c>
+      <c r="AV9" t="n">
+        <v>48.66</v>
+      </c>
+      <c r="AW9" t="n">
+        <v>350</v>
+      </c>
+      <c r="AX9" t="n">
+        <v>0</v>
+      </c>
+      <c r="AY9" t="n">
+        <v>10</v>
+      </c>
+      <c r="AZ9" t="n">
+        <v>222</v>
+      </c>
+      <c r="BA9" t="n">
+        <v>40</v>
+      </c>
+      <c r="BB9" t="n">
+        <v>40</v>
+      </c>
+      <c r="BC9" t="n">
+        <v>8</v>
+      </c>
+      <c r="BD9" t="n">
+        <v>28</v>
+      </c>
+      <c r="BE9" t="n">
+        <v>2.05</v>
+      </c>
+      <c r="BF9" t="n">
+        <v>4.07</v>
+      </c>
+      <c r="BG9" t="n">
         <v>0.4</v>
       </c>
-      <c r="BO2" t="n">
-        <v>21.4</v>
-      </c>
-      <c r="BP2" t="n">
-        <v>0</v>
-      </c>
-      <c r="BQ2" t="n">
-        <v>1.8</v>
-      </c>
-      <c r="BR2" t="n">
-        <v>2.2</v>
-      </c>
-      <c r="BS2" t="n">
-        <v>3.6</v>
+      <c r="BH9" t="n">
+        <v>7.73</v>
+      </c>
+      <c r="BI9" t="n">
+        <v>19.53</v>
+      </c>
+      <c r="BJ9" t="n">
+        <v>21.06</v>
+      </c>
+      <c r="BK9" t="n">
+        <v>3.24</v>
+      </c>
+      <c r="BL9" t="n">
+        <v>23.33</v>
+      </c>
+      <c r="BM9" t="n">
+        <v>0</v>
+      </c>
+      <c r="BN9" t="n">
+        <v>0.67</v>
+      </c>
+      <c r="BO9" t="n">
+        <v>14.8</v>
+      </c>
+      <c r="BP9" t="n">
+        <v>2.67</v>
+      </c>
+      <c r="BQ9" t="n">
+        <v>2.67</v>
+      </c>
+      <c r="BR9" t="n">
+        <v>0.53</v>
+      </c>
+      <c r="BS9" t="n">
+        <v>1.87</v>
       </c>
     </row>
   </sheetData>

</xml_diff>